<commit_message>
TC19 Updated for ECTEST
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC19_Verify_ShippingMethod.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC19_Verify_ShippingMethod.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF9551D-4F37-4E67-8835-1F658E82CECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DAD472-BCB3-45E6-86EA-8ED0EF2B1D99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="98">
   <si>
     <t>TestCase</t>
   </si>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1367,82 +1367,76 @@
     <row r="46" spans="1:5">
       <c r="A46" s="3"/>
       <c r="B46" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>75</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3"/>
-      <c r="B47" s="5" t="s">
-        <v>97</v>
+      <c r="B47" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E47" s="3"/>
+      <c r="E47" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3"/>
-      <c r="B48" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="B48" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3"/>
       <c r="B49" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="E49" s="3"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3"/>
-      <c r="B50" s="5" t="s">
-        <v>13</v>
+      <c r="B50" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E50" s="3"/>
+      <c r="E50" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3"/>
       <c r="B51" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3"/>
@@ -1450,12 +1444,27 @@
         <v>9</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="3"/>
+      <c r="B53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="D53" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1891,12 +1900,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -2093,6 +2096,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
@@ -2102,15 +2111,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2127,4 +2127,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>